<commit_message>
Alterações Relatórios Arquitetura Computacional
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
+++ b/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner Lucas\Desktop\Ferbgam\Sprint 2\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96d8cb575939bb1d/Desktop/Ferbgam/Sprint 2/Documentação/Relatório de Arq. Comp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4576EE2-C225-42A5-B5BD-629A5852060F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{C4576EE2-C225-42A5-B5BD-629A5852060F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9962C477-E8DC-479A-B94E-1C112E0C2AB9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="6" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros de temperatura" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Parametros de luminosidade" sheetId="3" r:id="rId3"/>
     <sheet name="Classificação temp - verao" sheetId="4" r:id="rId4"/>
     <sheet name="Classificação temp - inverno" sheetId="5" r:id="rId5"/>
-    <sheet name="Classificação de luminosidade" sheetId="7" r:id="rId6"/>
-    <sheet name="DHT11" sheetId="8" r:id="rId7"/>
-    <sheet name="LDR" sheetId="9" r:id="rId8"/>
+    <sheet name="Planilha2" sheetId="11" r:id="rId6"/>
+    <sheet name="Classificação de luminosidade" sheetId="7" r:id="rId7"/>
+    <sheet name="DHT11" sheetId="8" r:id="rId8"/>
+    <sheet name="LDR" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Temperatura</t>
   </si>
@@ -109,9 +110,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Crítico</t>
-  </si>
-  <si>
     <t>ideal</t>
   </si>
   <si>
@@ -209,6 +207,15 @@
   </si>
   <si>
     <t>-30°C a 70°C</t>
+  </si>
+  <si>
+    <t>Umidade %</t>
+  </si>
+  <si>
+    <t>Temperatura Verão °C</t>
+  </si>
+  <si>
+    <t>Temperatura Inverno °C</t>
   </si>
 </sst>
 </file>
@@ -218,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +276,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -309,19 +330,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF2929"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,6 +343,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -402,16 +423,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,9 +460,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -480,15 +495,40 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,6 +549,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>118745</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>62230</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="Tela de computador com texto preto sobre fundo branco&#10;&#10;Descrição gerada automaticamente com confiança média">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49B038F5-E8D1-4726-B043-307235E66B4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="971550"/>
+          <a:ext cx="2604770" cy="2395855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,24 +919,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="31"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="D3" s="28"/>
+      <c r="F3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
@@ -869,23 +967,23 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <f>QUARTILE(D8:D9,1)</f>
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <f>QUARTILE(D8:D9,3)</f>
         <v>23</v>
       </c>
@@ -916,10 +1014,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
@@ -959,10 +1057,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="30"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
@@ -992,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953A5C2A-4A23-4CD0-BFA1-81587011CDF4}">
   <dimension ref="C2:O25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1013,297 +1111,297 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="33"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="3:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="K3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="K3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="G4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="14">
         <v>20.399999999999999</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>20</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
         <f>_xlfn.QUARTILE.EXC(L4:L16,1)</f>
         <v>22.25</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <f>AVERAGE(L4:L16)</f>
         <v>23.299999999999997</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <f>MEDIAN(L4:L16)</f>
         <v>23</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <f>_xlfn.QUARTILE.EXC(L4:L16,3)</f>
         <v>23.75</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="22">
         <v>24</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <v>0.375</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>25</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="15">
         <v>22.2</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="K7" s="14">
+      <c r="D7" s="32"/>
+      <c r="K7" s="13">
         <v>0.45833333333333298</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="15">
         <v>22.9</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="K8" s="14">
+      <c r="D8" s="33"/>
+      <c r="K8" s="13">
         <v>0.5</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="15">
         <v>23.8</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <v>20</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <v>0.54166666666666696</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="15">
         <v>30</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="22">
         <v>24</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <v>0.58333333333333304</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="15">
         <v>23.7</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <v>0.625</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>23.1</v>
       </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="14">
+      <c r="K12" s="13">
         <v>0.66666666666666696</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="15">
         <v>22.5</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K13" s="14">
+      <c r="K13" s="13">
         <v>0.70833333333333304</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="15">
         <v>23</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K14" s="14">
+      <c r="K14" s="13">
         <v>0.75</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="15">
         <v>22.3</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
     </row>
     <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K15" s="14">
+      <c r="K15" s="13">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="16">
         <v>21</v>
       </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K16" s="14">
+      <c r="K16" s="13">
         <v>0.83333333333333304</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="15">
         <v>23</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
     </row>
     <row r="17" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
     </row>
     <row r="18" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
     </row>
     <row r="19" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
     </row>
     <row r="24" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
     </row>
     <row r="25" spans="11:15" x14ac:dyDescent="0.2">
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1321,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B3560A-DF5A-4298-B5B8-001401938B52}">
   <dimension ref="C2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1341,110 +1439,110 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="33"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="K3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="K3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="36"/>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="14">
         <v>23.4</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>23</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <f>_xlfn.QUARTILE.EXC(L4:L16,1)</f>
         <v>23.05</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <f>AVERAGE(L4:L16)</f>
         <v>23.507692307692306</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <f>MEDIAN(L4:L16)</f>
         <v>23.7</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <f>_xlfn.QUARTILE.EXC(L4:L16,3)</f>
         <v>24</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>26</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <v>0.375</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="15">
         <v>22.2</v>
       </c>
     </row>
     <row r="7" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="K7" s="14">
+      <c r="E7" s="29"/>
+      <c r="K7" s="13">
         <v>0.45833333333333298</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="15">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="K8" s="14">
+      <c r="E8" s="28"/>
+      <c r="K8" s="13">
         <v>0.5</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="15">
         <v>23.8</v>
       </c>
     </row>
@@ -1455,10 +1553,10 @@
       <c r="E9" s="3">
         <v>23</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <v>0.54166666666666696</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="15">
         <v>23.9</v>
       </c>
     </row>
@@ -1469,58 +1567,58 @@
       <c r="E10" s="4">
         <v>26</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <v>0.58333333333333304</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="15">
         <v>23.7</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <v>0.625</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>23.1</v>
       </c>
     </row>
     <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="14">
+      <c r="K12" s="13">
         <v>0.66666666666666696</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="15">
         <v>23.5</v>
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K13" s="14">
+      <c r="K13" s="13">
         <v>0.70833333333333304</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="15">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K14" s="14">
+      <c r="K14" s="13">
         <v>0.75</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="15">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K15" s="14">
+      <c r="K15" s="13">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="16">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K16" s="14">
+      <c r="K16" s="13">
         <v>0.83333333333333304</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="15">
         <v>24</v>
       </c>
     </row>
@@ -1533,15 +1631,165 @@
     <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A2E38F-B8F4-4D16-B9D2-FEC1FC4C1DB2}">
+  <dimension ref="J7:U14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="J7" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+    </row>
+    <row r="8" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="36"/>
+      <c r="N8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="8">
+        <v>40</v>
+      </c>
+      <c r="K9" s="8">
+        <v>43.1</v>
+      </c>
+      <c r="L9" s="20">
+        <v>51.23</v>
+      </c>
+      <c r="M9" s="20">
+        <v>53.5</v>
+      </c>
+      <c r="N9" s="8">
+        <v>58.3</v>
+      </c>
+      <c r="O9" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
+    </row>
+    <row r="13" spans="10:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="42"/>
+      <c r="N13" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="42"/>
+      <c r="T13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" s="41"/>
+    </row>
+    <row r="14" spans="10:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="39">
+        <v>40</v>
+      </c>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39">
+        <v>43.1</v>
+      </c>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39">
+        <v>51.23</v>
+      </c>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39">
+        <v>53.5</v>
+      </c>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39">
+        <v>58.3</v>
+      </c>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39">
+        <v>60</v>
+      </c>
+      <c r="U14" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="J12:U12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B850F594-B86B-402A-A397-D688B5BE6106}">
-  <dimension ref="B3:M17"/>
+  <dimension ref="B3:O17"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1559,167 +1807,168 @@
     <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="L3" s="33" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="L3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="33"/>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="36"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="M4" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
         <v>500</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <f>_xlfn.QUARTILE.EXC(M5:M17,1)</f>
         <v>515</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <f>AVERAGE(M5:M17)</f>
         <v>655.38461538461536</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <f>MEDIAN(M5:M17)</f>
         <v>680</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <f>_xlfn.QUARTILE.EXC(M5:M17,3)</f>
         <v>780</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>1000</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L6" s="14">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="13">
         <v>0.375</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="15">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L7" s="14">
+      <c r="O6" s="45"/>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="13">
         <v>0.41666666666666702</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L8" s="14">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="13">
         <v>0.45833333333333298</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="15">
         <v>530</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L9" s="14">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="13">
         <v>0.5</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="15">
         <v>620</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L10" s="14">
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="13">
         <v>0.54166666666666696</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="15">
         <v>650</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L11" s="14">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="13">
         <v>0.58333333333333304</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="15">
         <v>700</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L12" s="14">
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="13">
         <v>0.625</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="15">
         <v>780</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L13" s="14">
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="13">
         <v>0.66666666666666696</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="15">
         <v>985</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="14">
+    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="13">
         <v>0.70833333333333304</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="15">
         <v>815</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L15" s="14">
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="13">
         <v>0.75</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L16" s="14">
+    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="13">
         <v>0.79166666666666696</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="16">
         <v>680</v>
       </c>
     </row>
     <row r="17" spans="12:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L17" s="14">
+      <c r="L17" s="13">
         <v>0.83333333333333304</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="15">
         <v>780</v>
       </c>
     </row>
@@ -1733,7 +1982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10161843-187F-4ED8-9D31-02F511B8CB4B}">
   <dimension ref="C3:J16"/>
   <sheetViews>
@@ -1743,104 +1992,104 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="27"/>
-    <col min="3" max="3" width="28.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="2" width="9.140625" style="25"/>
+    <col min="3" max="3" width="28.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="37"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="D10" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="D12" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="38"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="27" t="s">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="38"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="D13" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="27" t="s">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="25" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1854,82 +2103,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D961D34-E278-4BF1-953C-40D78D40C64D}">
   <dimension ref="C3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="27"/>
-    <col min="3" max="3" width="41" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="2" width="9.140625" style="25"/>
+    <col min="3" max="3" width="41" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="37"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="27" t="s">
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="27" t="s">
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="27" t="s">
+      <c r="D6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="27" t="s">
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="27" t="s">
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="28" t="s">
+      <c r="D8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="27" t="s">
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="27" t="s">
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="25" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1941,21 +2190,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D47DF97F5812C48AC56EEAD13F91A14" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0c4349b4016a3368b0684d72c1ba297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="50b162ea5db14ab2c84d7999098f8f4b" ns3:_="">
     <xsd:import namespace="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
@@ -2101,31 +2335,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{882FB3DB-5FF2-4F59-A0CA-10C60ECEB173}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85882A-30F2-4429-8714-EB68B1387E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2141,4 +2366,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{882FB3DB-5FF2-4F59-A0CA-10C60ECEB173}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finalização dos PPT e Criação da Dashboard Estática
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
+++ b/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner Lucas\Desktop\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gm888\Documents\Repositorios\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B72DA67-0773-4F83-A720-C84CBE15CD13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4549FB-0225-422C-A448-D8099AEC707F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros de Leitura" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +314,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,74 +455,86 @@
     <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,6 +545,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0099"/>
       <color rgb="FFFF2929"/>
     </mruColors>
   </colors>
@@ -826,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FBEE08-D238-4305-A1AB-4004EB763B4F}">
-  <dimension ref="C2:G11"/>
+  <dimension ref="C2:G9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -841,82 +872,80 @@
     <col min="8" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="D2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="3:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="3:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="14" t="s">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="D4" s="24"/>
+      <c r="F4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="7" spans="3:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
+      <c r="G4" s="24"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="F7" s="15" t="s">
+      <c r="D7" s="22"/>
+      <c r="F7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="3:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="F8" s="13" t="s">
+      <c r="D8" s="23"/>
+      <c r="F8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="3:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="14" t="s">
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="D9" s="24"/>
+      <c r="F9" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="3:7" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="3:7" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="G9" s="24"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -948,20 +977,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="18"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="3:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
       <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
@@ -979,10 +1008,10 @@
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1000,14 +1029,14 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="19">
+      <c r="C5" s="12">
         <v>8</v>
       </c>
       <c r="D5" s="11">
         <f>QUARTILE(D9:D10,1)</f>
         <v>16</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="13">
         <v>20</v>
       </c>
       <c r="F5" s="11">
@@ -1017,7 +1046,7 @@
         <f>QUARTILE(D9:D10,3)</f>
         <v>32</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="13">
         <v>40</v>
       </c>
       <c r="K5" s="6">
@@ -1042,10 +1071,10 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="29"/>
       <c r="K7" s="6">
         <v>0.45833333333333298</v>
       </c>
@@ -1057,10 +1086,10 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="30"/>
       <c r="K8" s="6">
         <v>0.5</v>
       </c>
@@ -1072,10 +1101,10 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="12">
         <v>8</v>
       </c>
       <c r="G9" s="9"/>
@@ -1090,10 +1119,10 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="13">
         <v>40</v>
       </c>
       <c r="G10" s="9"/>
@@ -1119,10 +1148,10 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="25"/>
       <c r="K12" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1136,10 +1165,10 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="23"/>
       <c r="K13" s="6">
         <v>0.70833333333333304</v>
       </c>
@@ -1151,10 +1180,10 @@
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="24"/>
       <c r="K14" s="6">
         <v>0.75</v>
       </c>
@@ -1268,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B3560A-DF5A-4298-B5B8-001401938B52}">
-  <dimension ref="C2:L16"/>
+  <dimension ref="C1:L16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,21 +1318,24 @@
     <col min="13" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="18" t="s">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D1" s="39"/>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="18"/>
-    </row>
-    <row r="3" spans="3:12" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27" t="s">
+      <c r="L2" s="27"/>
+    </row>
+    <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1311,21 +1343,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="K4" s="5">
@@ -1335,15 +1367,15 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="5" spans="3:12" s="10" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="19">
+    <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="12">
         <v>5</v>
       </c>
       <c r="D5" s="11">
         <f>QUARTILE(E9:E10,1)</f>
         <v>13.25</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="13">
         <v>23</v>
       </c>
       <c r="F5" s="11">
@@ -1353,7 +1385,7 @@
         <f>QUARTILE(E9:E10,3)</f>
         <v>29.75</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="13">
         <v>38</v>
       </c>
       <c r="K5" s="6">
@@ -1363,7 +1395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K6" s="6">
         <v>0.41666666666666702</v>
       </c>
@@ -1371,11 +1403,11 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="7" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="28" t="s">
+    <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="32"/>
       <c r="K7" s="6">
         <v>0.45833333333333298</v>
       </c>
@@ -1383,11 +1415,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="25" t="s">
+    <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="30"/>
       <c r="K8" s="6">
         <v>0.5</v>
       </c>
@@ -1395,11 +1427,11 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="9" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="23" t="s">
+    <row r="9" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="13">
         <v>5</v>
       </c>
       <c r="K9" s="6">
@@ -1409,11 +1441,11 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="10" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="24" t="s">
+    <row r="10" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="12">
         <v>38</v>
       </c>
       <c r="K10" s="6">
@@ -1423,7 +1455,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="11" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K11" s="6">
         <v>0.625</v>
       </c>
@@ -1431,11 +1463,11 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="12" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="12" t="s">
+    <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="25"/>
       <c r="K12" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1443,11 +1475,11 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="13" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="13" t="s">
+    <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="23"/>
       <c r="K13" s="6">
         <v>0.70833333333333304</v>
       </c>
@@ -1455,11 +1487,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="14" t="s">
+    <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="24"/>
       <c r="K14" s="6">
         <v>0.75</v>
       </c>
@@ -1467,7 +1499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="6">
         <v>0.79166666666666696</v>
       </c>
@@ -1475,7 +1507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="3:12" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K16" s="6">
         <v>0.83333333333333304</v>
       </c>
@@ -1503,7 +1535,7 @@
   <dimension ref="C2:L16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,20 +1554,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="18"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1544,20 +1576,20 @@
       </c>
     </row>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="K4" s="5">
@@ -1568,7 +1600,7 @@
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="19">
+      <c r="C5" s="12">
         <f>E8</f>
         <v>10</v>
       </c>
@@ -1576,7 +1608,7 @@
         <f>QUARTILE(E8:E9,1)</f>
         <v>30</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="13">
         <v>40</v>
       </c>
       <c r="F5" s="11">
@@ -1586,7 +1618,7 @@
         <f>QUARTILE(E8:E9,3)</f>
         <v>70</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="13">
         <f>E9</f>
         <v>90</v>
       </c>
@@ -1606,10 +1638,10 @@
       </c>
     </row>
     <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="30"/>
       <c r="K7" s="6">
         <v>0.45833333333333298</v>
       </c>
@@ -1618,10 +1650,10 @@
       </c>
     </row>
     <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="13">
         <v>10</v>
       </c>
       <c r="K8" s="6">
@@ -1632,10 +1664,10 @@
       </c>
     </row>
     <row r="9" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="13">
         <v>90</v>
       </c>
       <c r="K9" s="6">
@@ -1654,10 +1686,10 @@
       </c>
     </row>
     <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="22"/>
       <c r="K11" s="6">
         <v>0.625</v>
       </c>
@@ -1666,10 +1698,10 @@
       </c>
     </row>
     <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="33"/>
       <c r="K12" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1678,10 +1710,10 @@
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="24"/>
       <c r="K13" s="6">
         <v>0.70833333333333304</v>
       </c>
@@ -1732,7 +1764,7 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,34 +1784,34 @@
   <sheetData>
     <row r="2" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="L3" s="18" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="L3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="18"/>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="36" t="s">
         <v>54</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1836,10 +1868,10 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="22"/>
       <c r="L8" s="6">
         <v>0.45833333333333298</v>
       </c>
@@ -1848,10 +1880,10 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="33"/>
       <c r="L9" s="6">
         <v>0.5</v>
       </c>
@@ -1860,10 +1892,10 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="24"/>
       <c r="L10" s="6">
         <v>0.54166666666666696</v>
       </c>
@@ -1880,10 +1912,10 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="32"/>
       <c r="L12" s="6">
         <v>0.625</v>
       </c>
@@ -1892,10 +1924,10 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="30"/>
       <c r="L13" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1904,10 +1936,10 @@
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="13">
         <v>200</v>
       </c>
       <c r="L14" s="6">
@@ -1918,10 +1950,10 @@
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="12">
         <v>1200</v>
       </c>
       <c r="L15" s="6">
@@ -1979,92 +2011,92 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2100,64 +2132,64 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2170,18 +2202,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2331,6 +2363,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{882FB3DB-5FF2-4F59-A0CA-10C60ECEB173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2342,14 +2382,6 @@
     <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Alterando os parâmetros analytics
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
+++ b/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gm888\Documents\Repositorios\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner Lucas\Desktop\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4549FB-0225-422C-A448-D8099AEC707F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD13E2F-A6AC-47C7-BBC2-992237C6D52F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros de Leitura" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>Temperatura</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Umidade</t>
   </si>
   <si>
-    <t>Alerta</t>
-  </si>
-  <si>
     <t>Ideal</t>
   </si>
   <si>
@@ -204,10 +201,28 @@
     <t>Entre 500 e 1000 lux</t>
   </si>
   <si>
-    <t>Crítico</t>
-  </si>
-  <si>
     <t>Umidade (% UR)</t>
+  </si>
+  <si>
+    <t>Extremamente baixa</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Extremamente alta</t>
+  </si>
+  <si>
+    <t>Temperatura °C - Inverno</t>
+  </si>
+  <si>
+    <t>Temperatura °C - Verão</t>
+  </si>
+  <si>
+    <t>Luminosidade (Lux)</t>
   </si>
 </sst>
 </file>
@@ -265,12 +280,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -295,12 +304,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF2929"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -308,18 +311,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,8 +326,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBB33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8800"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF2501"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -416,22 +431,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -452,25 +513,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -480,25 +538,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -507,34 +565,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,6 +618,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFBB33"/>
+      <color rgb="FFFFFF25"/>
+      <color rgb="FFFF2501"/>
+      <color rgb="FFFF8800"/>
+      <color rgb="FFFFFF05"/>
+      <color rgb="FFCC0000"/>
+      <color rgb="FF007E33"/>
+      <color rgb="FFFF4444"/>
       <color rgb="FFCC0099"/>
       <color rgb="FFFF2929"/>
     </mruColors>
@@ -865,87 +946,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="10"/>
-    <col min="4" max="4" width="22.42578125" style="10" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="25" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="3" width="9.140625" style="8"/>
+    <col min="4" max="4" width="22.42578125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="8"/>
+    <col min="7" max="7" width="25" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="25"/>
+      <c r="D2" s="20"/>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="F3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="F3" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="21"/>
+      <c r="F4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="F7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="24"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="F7" s="21" t="s">
+      <c r="D9" s="21"/>
+      <c r="F9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="F8" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -956,328 +1037,328 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953A5C2A-4A23-4CD0-BFA1-81587011CDF4}">
   <dimension ref="C2:O25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="10"/>
-    <col min="11" max="11" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="22.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="8"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="3:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="3" spans="3:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="26" t="s">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L4" s="5">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="33">
         <v>8</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L4" s="7">
-        <v>20</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="12">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="D5" s="36">
         <f>QUARTILE(D9:D10,1)</f>
         <v>16</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="34">
         <v>20</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="35">
         <v>24</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="36">
         <f>QUARTILE(D9:D10,3)</f>
         <v>32</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="33">
         <v>40</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>0.375</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>23.2</v>
       </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
     </row>
     <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>22.2</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="K7" s="6">
+      <c r="C7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="6">
         <v>22.9</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="K8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="6">
+        <v>23.8</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
         <v>8</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="K8" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="8">
-        <v>23.8</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="12">
-        <v>8</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="K9" s="6">
+      <c r="G9" s="7"/>
+      <c r="K9" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="6">
         <v>21</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <v>40</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="K10" s="6">
+      <c r="G10" s="7"/>
+      <c r="K10" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="6">
         <v>23.7</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="6">
+      <c r="K11" s="4">
         <v>0.625</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="6">
         <v>24</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="K12" s="6">
+      <c r="C12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="6">
         <v>22.5</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="M12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="K13" s="4">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="L13" s="6">
+        <v>23</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="K13" s="6">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="L13" s="8">
+      <c r="D14" s="21"/>
+      <c r="K14" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="6">
+        <v>22.3</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="4">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="L15" s="7">
+        <v>21</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="L16" s="6">
         <v>23</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="K14" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="L14" s="8">
-        <v>22.3</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="6">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="L15" s="9">
-        <v>21</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="6">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="L16" s="8">
-        <v>23</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
     </row>
     <row r="17" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
     </row>
     <row r="18" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
     </row>
     <row r="19" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
     <row r="20" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
     <row r="21" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
     </row>
     <row r="23" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
     </row>
     <row r="25" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1297,224 +1378,226 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B3560A-DF5A-4298-B5B8-001401938B52}">
-  <dimension ref="C1:L16"/>
+  <dimension ref="C1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="16.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="10"/>
-    <col min="11" max="11" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="9.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="8"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D1" s="39"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="27"/>
+      <c r="K2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>8</v>
+      <c r="C3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L4" s="5">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="33">
         <v>5</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L4" s="7">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="12">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="D5" s="36">
         <f>QUARTILE(E9:E10,1)</f>
         <v>13.25</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="34">
         <v>23</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="35">
         <v>26</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="36">
         <f>QUARTILE(E9:E10,3)</f>
         <v>29.75</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="33">
         <v>38</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>0.375</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>22.2</v>
       </c>
     </row>
     <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="32"/>
-      <c r="K7" s="6">
+      <c r="D7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="K8" s="6">
+      <c r="E8" s="27"/>
+      <c r="K8" s="4">
         <v>0.5</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>23.8</v>
       </c>
     </row>
     <row r="9" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>5</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="6">
         <v>23.9</v>
       </c>
     </row>
     <row r="10" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>38</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="6">
         <v>23.7</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="6">
+      <c r="K11" s="4">
         <v>0.625</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="6">
         <v>23.1</v>
       </c>
     </row>
     <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="25"/>
-      <c r="K12" s="6">
+      <c r="D12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="6">
         <v>23.5</v>
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="K13" s="6">
+      <c r="D13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="K13" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="K14" s="6">
+      <c r="D14" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="K14" s="4">
         <v>0.75</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="6">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="6">
+      <c r="K15" s="4">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="7">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="6">
+      <c r="K16" s="4">
         <v>0.83333333333333304</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="6">
         <v>24</v>
       </c>
     </row>
+    <row r="18" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D12:E12"/>
@@ -1527,6 +1610,7 @@
     <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1534,214 +1618,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AD2AE0-4CA2-4D9A-84D4-DDB50E233387}">
   <dimension ref="C2:L16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="16.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="10"/>
-    <col min="11" max="11" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="22.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="8"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="27"/>
+      <c r="K2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="38" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="38"/>
-      <c r="G4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="G4" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="12">
-        <f>E8</f>
+      <c r="C5" s="33">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="36">
         <f>QUARTILE(E8:E9,1)</f>
         <v>30</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="34">
         <v>40</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="35">
         <v>60</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="36">
         <f>QUARTILE(E8:E9,3)</f>
         <v>70</v>
       </c>
-      <c r="H5" s="13">
-        <f>E9</f>
+      <c r="H5" s="33">
         <v>90</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <v>0.375</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="K7" s="6">
+      <c r="E7" s="27"/>
+      <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="6">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>10</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="4">
         <v>0.5</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>90</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="6">
         <v>45.2</v>
       </c>
     </row>
     <row r="10" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="6">
+      <c r="K10" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="K11" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="L11" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="K11" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="L11" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="33"/>
-      <c r="K12" s="6">
+      <c r="E12" s="30"/>
+      <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="6">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="24"/>
-      <c r="K13" s="6">
+      <c r="D13" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="K13" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="6">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="6">
+      <c r="K14" s="4">
         <v>0.75</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="6">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="6">
+      <c r="K15" s="4">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="7">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="6">
+      <c r="K16" s="4">
         <v>0.83333333333333304</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="6">
         <v>58</v>
       </c>
     </row>
@@ -1763,219 +1845,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B850F594-B86B-402A-A397-D688B5BE6106}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="10.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="12" style="10" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="10"/>
-    <col min="12" max="12" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="22.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="8"/>
+    <col min="12" max="12" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="L3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="27"/>
+      <c r="B3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="L3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>13</v>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11">
-        <f>C14</f>
+      <c r="B5" s="10">
         <v>200</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="36">
         <f>QUARTILE(C14:C15,1)</f>
         <v>450</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="34">
         <v>500</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="35">
         <v>1000</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="36">
         <f>QUARTILE(C14:C15,3)</f>
         <v>950</v>
       </c>
-      <c r="G5" s="11">
-        <f>C15</f>
+      <c r="G5" s="9">
         <v>1200</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="5">
         <v>500</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="6">
+      <c r="L6" s="4">
         <v>0.375</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="6">
         <v>300</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L7" s="6">
+      <c r="L7" s="4">
         <v>0.41666666666666702</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="6">
         <v>400</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="L8" s="4">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="M8" s="6">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="L9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="6">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="L8" s="6">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="M8" s="8">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="L9" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="M9" s="8">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="L10" s="6">
+      <c r="C10" s="21"/>
+      <c r="L10" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="6">
         <v>650</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L11" s="6">
+      <c r="L11" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="6">
         <v>700</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="L12" s="6">
+      <c r="B12" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="L12" s="4">
         <v>0.625</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="6">
         <v>780</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="L13" s="6">
+      <c r="C13" s="27"/>
+      <c r="L13" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="6">
         <v>985</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="10">
         <v>200</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="6">
         <v>815</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <v>1200</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="4">
         <v>0.75</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="6">
         <v>780</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L16" s="6">
+      <c r="L16" s="4">
         <v>0.79166666666666696</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <v>680</v>
       </c>
     </row>
     <row r="17" spans="12:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L17" s="6">
+      <c r="L17" s="4">
         <v>0.83333333333333304</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17" s="6">
         <v>780</v>
       </c>
     </row>
@@ -2004,105 +2084,105 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="28.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="28.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="34"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="D10" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="35"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="18" t="s">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="35"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="D13" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="18" t="s">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="10" t="s">
-        <v>12</v>
+      <c r="J16" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2125,72 +2205,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="41" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="41" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="34"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="18" t="s">
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="18" t="s">
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="18" t="s">
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="18" t="s">
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="19" t="s">
+      <c r="D8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="18" t="s">
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="18" t="s">
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2202,21 +2282,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D47DF97F5812C48AC56EEAD13F91A14" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0c4349b4016a3368b0684d72c1ba297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="50b162ea5db14ab2c84d7999098f8f4b" ns3:_="">
     <xsd:import namespace="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
@@ -2362,10 +2427,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85882A-30F2-4429-8714-EB68B1387E54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2387,19 +2477,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85882A-30F2-4429-8714-EB68B1387E54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adicionando o Hexadecimal das cores analytics
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
+++ b/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner Lucas\Desktop\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD13E2F-A6AC-47C7-BBC2-992237C6D52F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1FA749-9B14-4FBE-A599-81841A7AE617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros de Leitura" sheetId="1" r:id="rId1"/>
@@ -541,19 +541,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -568,7 +595,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -581,33 +608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -618,10 +618,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF2501"/>
+      <color rgb="FFFF8800"/>
       <color rgb="FFFFBB33"/>
       <color rgb="FFFFFF25"/>
-      <color rgb="FFFF2501"/>
-      <color rgb="FFFF8800"/>
       <color rgb="FFFFFF05"/>
       <color rgb="FFCC0000"/>
       <color rgb="FF007E33"/>
@@ -954,79 +954,79 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="D3" s="29"/>
+      <c r="F3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="F4" s="21" t="s">
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="F7" s="22" t="s">
+      <c r="D7" s="28"/>
+      <c r="F7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="F8" s="19" t="s">
+      <c r="D8" s="29"/>
+      <c r="F8" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="F9" s="21" t="s">
+      <c r="D9" s="30"/>
+      <c r="F9" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1035,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953A5C2A-4A23-4CD0-BFA1-81587011CDF4}">
-  <dimension ref="C2:O25"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,21 +1057,21 @@
     <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="K2" s="24" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="24"/>
-    </row>
-    <row r="3" spans="3:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="L2" s="33"/>
+    </row>
+    <row r="3" spans="2:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1082,21 +1082,22 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="41" t="s">
+    <row r="4" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4"/>
+      <c r="C4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="25" t="s">
         <v>57</v>
       </c>
       <c r="K4" s="3">
@@ -1109,25 +1110,25 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="3:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="33">
+    <row r="5" spans="2:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="19">
         <v>8</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="22">
         <f>QUARTILE(D9:D10,1)</f>
         <v>16</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="20">
         <v>20</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="21">
         <v>24</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="22">
         <f>QUARTILE(D9:D10,3)</f>
         <v>32</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="19">
         <v>40</v>
       </c>
       <c r="K5" s="4">
@@ -1140,7 +1141,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K6" s="4">
         <v>0.41666666666666702</v>
       </c>
@@ -1151,11 +1152,11 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="25" t="s">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="35"/>
       <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
@@ -1166,11 +1167,11 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="36"/>
       <c r="K8" s="4">
         <v>0.5</v>
       </c>
@@ -1181,7 +1182,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="12" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1218,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K11" s="4">
         <v>0.625</v>
       </c>
@@ -1228,11 +1229,11 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="20" t="s">
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="31"/>
       <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
@@ -1245,11 +1246,11 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="19" t="s">
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="29"/>
       <c r="K13" s="4">
         <v>0.70833333333333304</v>
       </c>
@@ -1260,11 +1261,11 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="21" t="s">
+    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="30"/>
       <c r="K14" s="4">
         <v>0.75</v>
       </c>
@@ -1275,7 +1276,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="4">
         <v>0.79166666666666696</v>
       </c>
@@ -1286,7 +1287,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K16" s="4">
         <v>0.83333333333333304</v>
       </c>
@@ -1404,20 +1405,20 @@
       <c r="D1" s="18"/>
     </row>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="24"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1426,20 +1427,20 @@
       </c>
     </row>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="25" t="s">
         <v>57</v>
       </c>
       <c r="K4" s="3">
@@ -1450,24 +1451,24 @@
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="33">
+      <c r="C5" s="19">
         <v>5</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="22">
         <f>QUARTILE(E9:E10,1)</f>
         <v>13.25</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="20">
         <v>23</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="21">
         <v>26</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="22">
         <f>QUARTILE(E9:E10,3)</f>
         <v>29.75</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="19">
         <v>38</v>
       </c>
       <c r="K5" s="4">
@@ -1486,10 +1487,10 @@
       </c>
     </row>
     <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="38"/>
       <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
@@ -1498,10 +1499,10 @@
       </c>
     </row>
     <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="36"/>
       <c r="K8" s="4">
         <v>0.5</v>
       </c>
@@ -1546,10 +1547,10 @@
       </c>
     </row>
     <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="31"/>
       <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
@@ -1558,10 +1559,10 @@
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="19"/>
+      <c r="E13" s="29"/>
       <c r="K13" s="4">
         <v>0.70833333333333304</v>
       </c>
@@ -1570,10 +1571,10 @@
       </c>
     </row>
     <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="30"/>
       <c r="K14" s="4">
         <v>0.75</v>
       </c>
@@ -1638,20 +1639,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="24"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="3:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1660,20 +1661,20 @@
       </c>
     </row>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="25" t="s">
         <v>57</v>
       </c>
       <c r="K4" s="3">
@@ -1684,24 +1685,24 @@
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="33">
+      <c r="C5" s="19">
         <v>10</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="22">
         <f>QUARTILE(E8:E9,1)</f>
         <v>30</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="20">
         <v>40</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="21">
         <v>60</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="22">
         <f>QUARTILE(E8:E9,3)</f>
         <v>70</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="19">
         <v>90</v>
       </c>
       <c r="K5" s="4">
@@ -1720,10 +1721,10 @@
       </c>
     </row>
     <row r="7" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="36"/>
       <c r="K7" s="4">
         <v>0.45833333333333298</v>
       </c>
@@ -1768,10 +1769,10 @@
       </c>
     </row>
     <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="28"/>
       <c r="K11" s="4">
         <v>0.625</v>
       </c>
@@ -1780,10 +1781,10 @@
       </c>
     </row>
     <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="39"/>
       <c r="K12" s="4">
         <v>0.66666666666666696</v>
       </c>
@@ -1792,10 +1793,10 @@
       </c>
     </row>
     <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="30"/>
       <c r="K13" s="4">
         <v>0.70833333333333304</v>
       </c>
@@ -1845,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B850F594-B86B-402A-A397-D688B5BE6106}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1866,34 +1867,34 @@
   <sheetData>
     <row r="2" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="L3" s="24" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="L3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="25" t="s">
         <v>57</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -1907,17 +1908,17 @@
       <c r="B5" s="10">
         <v>200</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="22">
         <f>QUARTILE(C14:C15,1)</f>
         <v>450</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="20">
         <v>500</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="21">
         <v>1000</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="22">
         <f>QUARTILE(C14:C15,3)</f>
         <v>950</v>
       </c>
@@ -1948,10 +1949,10 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="28"/>
       <c r="L8" s="4">
         <v>0.45833333333333298</v>
       </c>
@@ -1960,10 +1961,10 @@
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="39"/>
       <c r="L9" s="4">
         <v>0.5</v>
       </c>
@@ -1972,10 +1973,10 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="30"/>
       <c r="L10" s="4">
         <v>0.54166666666666696</v>
       </c>
@@ -1992,10 +1993,10 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="38"/>
       <c r="L12" s="4">
         <v>0.625</v>
       </c>
@@ -2004,10 +2005,10 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="36"/>
       <c r="L13" s="4">
         <v>0.66666666666666696</v>
       </c>
@@ -2091,10 +2092,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
@@ -2121,10 +2122,10 @@
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="15" t="s">
@@ -2151,10 +2152,10 @@
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="15" t="s">
@@ -2212,10 +2213,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
@@ -2282,6 +2283,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D47DF97F5812C48AC56EEAD13F91A14" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0c4349b4016a3368b0684d72c1ba297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="50b162ea5db14ab2c84d7999098f8f4b" ns3:_="">
     <xsd:import namespace="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
@@ -2427,35 +2443,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85882A-30F2-4429-8714-EB68B1387E54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2477,9 +2468,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448DDDC1-C40D-4EA1-A682-89DC71B87F05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85882A-30F2-4429-8714-EB68B1387E54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2738bcf7-a7d1-483c-b8c3-3b8e485feb0d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrigindo a parte de luminosidade - analytics
</commit_message>
<xml_diff>
--- a/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
+++ b/Sprint 2/Documentação/Relatório de Arq. Comp/Tabela de parametros - arq comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner Lucas\Desktop\Ferbgam\Sprint 2\Documentação\Relatório de Arq. Comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A02789D-8BE4-4493-A249-98B6CB378A71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A941AF3D-1326-4697-B76D-B3B2EC18CC11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{F7AB22E7-DEF3-4CFB-ABB6-9665A6792E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros de Leitura" sheetId="1" r:id="rId1"/>
@@ -1048,7 +1048,7 @@
   <dimension ref="B2:O25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B3560A-DF5A-4298-B5B8-001401938B52}">
   <dimension ref="C1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AD2AE0-4CA2-4D9A-84D4-DDB50E233387}">
   <dimension ref="C2:L16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B850F594-B86B-402A-A397-D688B5BE6106}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1920,11 +1920,11 @@
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C5" s="22">
         <f>QUARTILE(C14:C15,1)</f>
-        <v>450</v>
+        <v>375</v>
       </c>
       <c r="D5" s="20">
         <v>500</v>
@@ -1934,10 +1934,10 @@
       </c>
       <c r="F5" s="22">
         <f>QUARTILE(C14:C15,3)</f>
-        <v>950</v>
+        <v>1125</v>
       </c>
       <c r="G5" s="9">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="L5" s="3">
         <v>0.33333333333333331</v>
@@ -2035,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="L14" s="4">
         <v>0.70833333333333304</v>
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="9">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="L15" s="4">
         <v>0.75</v>

</xml_diff>